<commit_message>
Added Test Scripts for Scenario - PCApp_TestScenario_007 and new Test Cases document
</commit_message>
<xml_diff>
--- a/Test Suite/UZ_Dilabs_SOS_Test Script_v_0.2.xlsx
+++ b/Test Suite/UZ_Dilabs_SOS_Test Script_v_0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srita\OneDrive\Dilabs\QA Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="102_{47737EB7-8A02-4037-B6CA-CC9AC3410C92}" revIDLastSave="611" xr10:uidLastSave="{C6EFCC25-7C23-4DD0-841D-17BBCCBE15A6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28"/>
+  <xr:revisionPtr documentId="102_{47737EB7-8A02-4037-B6CA-CC9AC3410C92}" revIDLastSave="613" xr10:uidLastSave="{4758975B-7DE9-49E2-9590-D87F8BE2FD48}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="786" windowHeight="9048" windowWidth="23040" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView activeTab="1" minimized="1" tabRatio="786" windowHeight="9048" windowWidth="23040" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestDetails" r:id="rId1" sheetId="3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
   <si>
     <t>PROJECT</t>
   </si>
@@ -287,7 +287,70 @@
     <t>EXECUTION STATUS</t>
   </si>
   <si>
+    <t>PCApp_TestCase_002_C15</t>
+  </si>
+  <si>
+    <t>Verify user can create minimum of 20 Profiles</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_005_PS05</t>
+  </si>
+  <si>
+    <t>Connect the USB UART to PC, launch the App and verify it is listed in the Port Dropdown list</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_005_PS06</t>
+  </si>
+  <si>
+    <t>Launch the PC App, and connect the USB UART to PC and verify it is listed in the Port Dropdown list</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_005_PS07</t>
+  </si>
+  <si>
+    <t>Remove the USB UART from the PC and verify the same is reflected in the Port Dropdown list</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_005_PS08</t>
+  </si>
+  <si>
+    <t>Connect multiple USB UART to PC, launch the App and verify all are listed in the Port Dropdown list</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_005_PS09</t>
+  </si>
+  <si>
+    <t>Connect USB devices like Pendrive, External Harddisak, launch the App and verify it is listed in the Port Dropdown list</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_002_AP03</t>
+  </si>
+  <si>
+    <t>Verify when user has created a new profile and click on close button to exit the Application, user is prompted to confirm the exit</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_002_AP04</t>
+  </si>
+  <si>
+    <t>Verify when user has selected a profile and click on close button to exit the Application, user is prompted to confirm the exit</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_002_AP05</t>
+  </si>
+  <si>
+    <t>Verify when user clicks on OK button on the exit dialog box the Application is closed</t>
+  </si>
+  <si>
+    <t>PCApp_TestCase_002_AP06</t>
+  </si>
+  <si>
+    <t>Verify when user clicks on the Cancel button on the exit dialog box, the user stays back at the same screen</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -974,7 +1037,7 @@
   <dimension ref="A1:D261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A44" sqref="A44:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,7 +1071,9 @@
       <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -1017,7 +1082,9 @@
       <c r="B4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -1026,7 +1093,9 @@
       <c r="B5" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -1035,7 +1104,9 @@
       <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -1044,7 +1115,9 @@
       <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
@@ -1053,7 +1126,9 @@
       <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
@@ -1062,7 +1137,9 @@
       <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
@@ -1071,7 +1148,9 @@
       <c r="B10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
@@ -1080,7 +1159,9 @@
       <c r="B11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
@@ -1098,7 +1179,9 @@
       <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
@@ -1107,7 +1190,9 @@
       <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
@@ -1116,7 +1201,9 @@
       <c r="B15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
@@ -1125,7 +1212,9 @@
       <c r="B16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
@@ -1134,7 +1223,9 @@
       <c r="B17" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
@@ -1143,7 +1234,9 @@
       <c r="B18" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
@@ -1152,241 +1245,319 @@
       <c r="B19" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C20" s="12"/>
     </row>
     <row customHeight="1" ht="45" r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>56</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="12"/>
+        <v>73</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="45" r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row customHeight="1" ht="45" r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row customHeight="1" ht="45" r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row customHeight="1" ht="45" r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C37" s="5"/>
     </row>
     <row customHeight="1" ht="45" r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="5"/>
+    </row>
+    <row customHeight="1" ht="49.95" r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="5"/>
+    </row>
+    <row customHeight="1" ht="49.95" r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="5"/>
+    </row>
+    <row customHeight="1" ht="49.95" r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="5"/>
+    </row>
+    <row customHeight="1" ht="49.95" r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="5"/>
+    </row>
+    <row customHeight="1" ht="49.95" r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="5"/>
+    </row>
+    <row customHeight="1" ht="49.95" r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row customHeight="1" ht="49.95" r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row customHeight="1" ht="49.95" r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row customHeight="1" ht="49.95" r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-    </row>
-    <row customHeight="1" ht="49.95" r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row customHeight="1" ht="49.95" r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-    </row>
-    <row customHeight="1" ht="49.95" r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
+      <c r="A45" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
+      <c r="A46" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
+      <c r="A47" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
+      <c r="A48" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>

</xml_diff>

<commit_message>
changed images as per new GUI, new APP 1.2.0.0 is added
</commit_message>
<xml_diff>
--- a/Test Suite/UZ_Dilabs_SOS_Test Script_v_0.2.xlsx
+++ b/Test Suite/UZ_Dilabs_SOS_Test Script_v_0.2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="103">
   <si>
     <t>PROJECT</t>
   </si>
@@ -1459,7 +1459,9 @@
       <c r="B39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row customHeight="1" ht="49.95" r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">

</xml_diff>